<commit_message>
Manger Screen and commenting code
</commit_message>
<xml_diff>
--- a/GenXServiceEngagementCenterApplication/AnalyticalReports/Top topics raised.xlsx
+++ b/GenXServiceEngagementCenterApplication/AnalyticalReports/Top topics raised.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>PROBLEM</t>
   </si>
@@ -20,30 +20,18 @@
     <t>Number Of Times Raised</t>
   </si>
   <si>
-    <t>word</t>
-  </si>
-  <si>
-    <t>OneNote</t>
+    <t>Microsoft Sway ended with an error is not able to open charts</t>
   </si>
   <si>
     <t>Microsoft OneNote ended with an error is taking too long to open</t>
   </si>
   <si>
-    <t>Microsoft Sway ended with an error is not able to open charts</t>
+    <t>Microsoft Power BI ended with an error is not able to start</t>
   </si>
   <si>
     <t>Microsoft OneNote ended with an error not able to start</t>
   </si>
   <si>
-    <t>Publisher is not able to work properly</t>
-  </si>
-  <si>
-    <t>publisher not working properly</t>
-  </si>
-  <si>
-    <t>Word</t>
-  </si>
-  <si>
     <t>Microsoft Office ended with an error is hanging</t>
   </si>
   <si>
@@ -74,9 +62,6 @@
     <t>Microsoft Excel ended with an error is hanging</t>
   </si>
   <si>
-    <t>publisher</t>
-  </si>
-  <si>
     <t>Microsoft Publisher ended with an error is not able to start</t>
   </si>
   <si>
@@ -90,15 +75,6 @@
   </si>
   <si>
     <t>Microsoft Project ended with an error is not able to connect to API</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Microsoft Power BI ended with an error is not able to start</t>
-  </si>
-  <si>
-    <t>PowerPoint not working</t>
   </si>
   <si>
     <t>Microsoft Access ended with an error is not able to open charts</t>
@@ -149,7 +125,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -168,7 +144,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="3">
@@ -184,7 +160,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="5">
@@ -192,7 +168,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="6">
@@ -328,70 +304,6 @@
         <v>22</v>
       </c>
       <c r="B22" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" t="n">
         <v>1.0</v>
       </c>
     </row>

</xml_diff>